<commit_message>
retrieve sheet dan read by sheet
</commit_message>
<xml_diff>
--- a/File/DOCTemplateDUmmy.xlsx
+++ b/File/DOCTemplateDUmmy.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f097b7bb5cf5ee08/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECT\SKY.RECOVERY.LOCAL\File\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{551CEB8E-B993-4D93-9659-667118DC8972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8C739A2-EB28-4D04-97DF-1F7EAD800B1B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24234E95-B647-4A76-909F-351F0FD3064B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{94BEB77D-EA06-4EB7-BE0F-8E34D40F12B8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{94BEB77D-EA06-4EB7-BE0F-8E34D40F12B8}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralMasterEmployee" sheetId="1" r:id="rId1"/>
+    <sheet name="GeneralMasterLoan" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="75">
   <si>
     <t>Id</t>
   </si>
@@ -211,6 +212,54 @@
   </si>
   <si>
     <t>Balikpapan</t>
+  </si>
+  <si>
+    <t>Nama Nasabah</t>
+  </si>
+  <si>
+    <t>Kota Tinggal</t>
+  </si>
+  <si>
+    <t>Jumlah Hutang</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Eko Patrio</t>
+  </si>
+  <si>
+    <t>Sumanto</t>
+  </si>
+  <si>
+    <t>Baharuddin</t>
+  </si>
+  <si>
+    <t>Suprapto</t>
+  </si>
+  <si>
+    <t>Raharjo</t>
+  </si>
+  <si>
+    <t>Bambang</t>
+  </si>
+  <si>
+    <t>Suminto</t>
+  </si>
+  <si>
+    <t>Ponaryo</t>
+  </si>
+  <si>
+    <t>Reza</t>
+  </si>
+  <si>
+    <t>Denpasar</t>
+  </si>
+  <si>
+    <t>Nunggak</t>
+  </si>
+  <si>
+    <t>DPD</t>
   </si>
 </sst>
 </file>
@@ -261,9 +310,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -581,7 +631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26830FA1-540B-403A-97A8-BAEA1FDA6099}">
   <dimension ref="A2:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -884,4 +934,244 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{721E0E56-798E-4790-A6A8-D2FB3EC25E9B}">
+  <dimension ref="A2:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="2">
+        <v>5000000</v>
+      </c>
+      <c r="E3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2500000</v>
+      </c>
+      <c r="E4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="2">
+        <v>3450000</v>
+      </c>
+      <c r="E5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="E6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="2">
+        <v>4300000</v>
+      </c>
+      <c r="E7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2100000</v>
+      </c>
+      <c r="E8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1450000</v>
+      </c>
+      <c r="E9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1200000</v>
+      </c>
+      <c r="E10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="2">
+        <v>450000</v>
+      </c>
+      <c r="E11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="2">
+        <v>500000</v>
+      </c>
+      <c r="E12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>